<commit_message>
Time adjusted in Sprints
Time for the separate springs adjusted
</commit_message>
<xml_diff>
--- a/Documentation/Sprints.xlsx
+++ b/Documentation/Sprints.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Item Type</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Bind the references needed for the Excel database driver</t>
   </si>
   <si>
-    <t>Implement a TabController with a DataGridView for Displaying the Data pulled from the DB</t>
-  </si>
-  <si>
     <t>Build a file choosing option for selecting the wanted Excel sheet, with limiting extension (.xls, xlsx)</t>
   </si>
   <si>
@@ -68,19 +65,25 @@
     <t>Handle all necessary CRUD operations with the DB, display results in a table.</t>
   </si>
   <si>
-    <t>Implement onClick generation of a new Tab with the detailed info of the clicked member in the table.</t>
-  </si>
-  <si>
     <t>Build a member info (new payment) update section in the detailed information Tab</t>
   </si>
   <si>
     <t>Implement the BackupManager, saving the file every 3 days and holding 10 versions at once.</t>
   </si>
   <si>
-    <t>Create Test class for Unit Tests</t>
-  </si>
-  <si>
     <t>Publish the Application</t>
+  </si>
+  <si>
+    <t>Time [h]</t>
+  </si>
+  <si>
+    <t>Implement onClick generation of a new Window with the detailed info of the clicked member in the table.</t>
+  </si>
+  <si>
+    <t>Implement a DataGridView for Displaying the Data pulled from the DB</t>
+  </si>
+  <si>
+    <t>Create Test class for Unit Tests (researche)</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -152,11 +155,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB1BBCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB1BBCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -165,6 +179,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -445,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +477,7 @@
     <col min="4" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,8 +487,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -480,8 +501,11 @@
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -491,8 +515,11 @@
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -502,8 +529,11 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -513,8 +543,11 @@
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -522,10 +555,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -533,43 +569,55 @@
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3">
-        <v>3</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3">
-        <v>3</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -577,10 +625,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -588,10 +639,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -599,10 +653,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -610,10 +667,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D14" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
@@ -621,10 +681,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D15" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
@@ -632,7 +695,16 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="5">
+        <f>SUM(D2:D16)</f>
+        <v>35.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Product Backlog images and updated Docu
Also rearanged a couple things,
</commit_message>
<xml_diff>
--- a/Documentation/Sprints.xlsx
+++ b/Documentation/Sprints.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smueller\Documents\GitHub\Excel-Administration\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Doe\Documents\GitHub\Excel-Administration\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Item Type</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Design Main User Interface</t>
   </si>
   <si>
-    <t>Create an alternative for closing the program via File -&gt; Exit</t>
-  </si>
-  <si>
     <t>Create a class that will handle all Database related actions.</t>
   </si>
   <si>
@@ -65,12 +62,6 @@
     <t>Handle all necessary CRUD operations with the DB, display results in a table.</t>
   </si>
   <si>
-    <t>Build a member info (new payment) update section in the detailed information Tab</t>
-  </si>
-  <si>
-    <t>Implement the BackupManager, saving the file every 3 days and holding 10 versions at once.</t>
-  </si>
-  <si>
     <t>Publish the Application</t>
   </si>
   <si>
@@ -83,7 +74,10 @@
     <t>Implement a DataGridView for Displaying the Data pulled from the DB</t>
   </si>
   <si>
-    <t>Create Test class for Unit Tests (researche)</t>
+    <t>Implement the BackupManager, making a Backup before each change in the DB.</t>
+  </si>
+  <si>
+    <t>Build a member info (new payment) update section in the detailed information Window</t>
   </si>
 </sst>
 </file>
@@ -185,7 +179,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -463,13 +457,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="2" bestFit="1" customWidth="1"/>
@@ -488,7 +482,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -516,7 +510,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="5">
-        <v>0.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -524,13 +518,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="5">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -541,10 +535,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D5" s="5">
-        <v>1</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -555,10 +549,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D6" s="5">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -566,13 +560,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="5">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -586,7 +580,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -608,13 +602,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="5">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -625,10 +619,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D11" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -642,7 +636,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="5">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,13 +644,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="5">
         <v>4</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="5">
-        <v>2.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -667,44 +661,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D14" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="3">
-        <v>5</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="3">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="D16" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="5">
-        <f>SUM(D2:D16)</f>
-        <v>35.5</v>
+        <f>SUM(D2:D14)</f>
+        <v>44.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pictures of separate Springs
Adjusted the Springs.xls table, missing some implemented features. Also
fixed hours.
</commit_message>
<xml_diff>
--- a/Documentation/Sprints.xlsx
+++ b/Documentation/Sprints.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Item Type</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Handle all necessary CRUD operations with the DB, display results in a table.</t>
   </si>
   <si>
-    <t>Publish the Application</t>
-  </si>
-  <si>
     <t>Time [h]</t>
   </si>
   <si>
@@ -78,6 +75,12 @@
   </si>
   <si>
     <t>Build a member info (new payment) update section in the detailed information Window</t>
+  </si>
+  <si>
+    <t>Implement removal of members form the DB</t>
+  </si>
+  <si>
+    <t>Implement the addition of a new Member in the Database via the New Member Window</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -510,7 +513,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="5">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -535,7 +538,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="5">
         <v>3.5</v>
@@ -608,7 +611,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -619,7 +622,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="5">
         <v>3</v>
@@ -633,7 +636,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="5">
         <v>2.5</v>
@@ -647,10 +650,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D13" s="5">
-        <v>4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -661,16 +664,30 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D14" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" s="5">
-        <f>SUM(D2:D14)</f>
-        <v>44.5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="5">
+        <f>SUM(D2:D15)</f>
+        <v>47.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Docu update with Development hours and tests
Format of the tests adjusted again.
Added a picture of the development hours
</commit_message>
<xml_diff>
--- a/Documentation/Sprints.xlsx
+++ b/Documentation/Sprints.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Doe\Documents\GitHub\Excel-Administration\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\Excel-Administration\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="840" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Item Type</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Implement the addition of a new Member in the Database via the New Member Window</t>
+  </si>
+  <si>
+    <t>Software development total time</t>
   </si>
 </sst>
 </file>
@@ -167,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -180,9 +183,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -462,11 +468,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="2" bestFit="1" customWidth="1"/>
@@ -684,7 +690,10 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D17" s="5">
         <f>SUM(D2:D15)</f>
         <v>47.5</v>

</xml_diff>